<commit_message>
Finish sms send function.
</commit_message>
<xml_diff>
--- a/src/main/webapp/upload/lottery.xlsx
+++ b/src/main/webapp/upload/lottery.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/projects/workspace-java/sms-demo/src/main/webapp/upload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwang02/workspace-java/sms-demo/src/main/webapp/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
   <si>
     <t>田友梅</t>
   </si>
@@ -236,26 +236,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，主办方已快递出礼品。收到活动主办方派送的礼品后，请当场确认是否完好。若发现异常请直接拒收，后续会安排重寄。若签收后发现礼品损坏，活动主办方不再补寄。特此短信告知，再次感谢您选购丝塔芙产品！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>丝塔芙] 感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761767的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761767的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>丝塔芙]感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，很遗憾，您提供的获奖信息及购物凭证未通过主办方审核，因此根据活动规则，将取消领奖资格。特此短信告知，敬请谅解！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，很遗憾，您提供的获奖信息及购物凭证未通过主办方审核，因此根据活动规则，将取消领奖资格。特此短信告知，敬请谅解！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>13917147923</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -347,9 +335,6 @@
     <t>15868373753</t>
   </si>
   <si>
-    <t>丝塔芙] 感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761767的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -504,6 +489,150 @@
   </si>
   <si>
     <t>18319952764</t>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，很遗憾，您提供的获奖信息及购物凭证未通过主办方审核，因此根据活动规则，将取消领奖资格。特此短信告知，敬请谅解！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，主办方已快递出礼品。收到活动主办方派送的礼品后，请当场确认是否完好。若发现异常请直接拒收，后续会安排重寄。若签收后发现礼品损坏，活动主办方不再补寄。特此短信告知，再次感谢您选购丝塔芙产品！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761767的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，主办方已快递出礼品。收到活动主办方派送的礼品后，请当场确认是否完好。若发现异常请直接拒收，后续会安排重寄。若签收后发现礼品损坏，活动主办方不再补寄。特此短信告知，再次感谢您选购丝塔芙产品！退订回N</t>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，很遗憾，您提供的获奖信息及购物凭证未通过主办方审核，因此根据活动规则，将取消领奖资格。特此短信告知，敬请谅解！退订回N</t>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761766的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761769的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761768的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761770的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761771的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761772的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761773的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761774的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761775的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761776的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761777的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761778的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761779的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761780的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761781的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761782的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761783的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761784的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761785的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761786的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761787的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761788的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761789的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，恭喜您抽中价值99元的mambo智能手环一份！因数次拨打您的电话，未能接通，特此短信告知。48小时内我们还会通过021-60761790的电话再次拨打该号码确认您的个人信息，请保持手机畅通。如仍旧联系不到您，则视为自动放弃本次机会。再次感谢您的参与！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢您参与“温和力量 焕出肌肤健康美”晒小票赢好礼活动，主办方已快递出礼品。收到活动主办方派送的礼品后，请当场确认是否完好。若发现异常请直接拒收，后续会安排重寄。若签收后发现礼品损坏，活动主办方不再补寄。特此短信告知，再次感谢您选购丝塔芙产品！退订回N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王义君</t>
+    <rPh sb="0" eb="1">
+      <t>wang'yi'jun</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13917147923</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -986,37 +1115,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="183.1640625" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1027,588 +1156,731 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="15"/>
-    <col min="3" max="3" width="20.33203125" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="8" style="15" customWidth="1"/>
+    <col min="2" max="2" width="10" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15" style="15" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>65</v>
+        <v>155</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1838,7 +2110,7 @@
         <v>15868373753</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -2186,7 +2458,7 @@
         <v>15705286084</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">

</xml_diff>